<commit_message>
In STR file, replaced example -> study1.
</commit_message>
<xml_diff>
--- a/metadata/STUDY1/STR-STUDY1.xlsx
+++ b/metadata/STUDY1/STR-STUDY1.xlsx
@@ -1,29 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/hadatac-example/metadata/STUDY1/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052BFA16-1BA0-DD48-A378-EEC148B67CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="16760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
-    <sheet name="FILESTREAM" sheetId="2" r:id="rId2"/>
-    <sheet name="MESSAGESTREAM" sheetId="3" r:id="rId3"/>
-    <sheet name="MESSAGETOPIC" sheetId="4" r:id="rId4"/>
+    <sheet name="InfoSheet" sheetId="1" r:id="rId4"/>
+    <sheet name="FILESTREAM" sheetId="2" r:id="rId5"/>
+    <sheet name="MESSAGESTREAM" sheetId="3" r:id="rId6"/>
+    <sheet name="MESSAGETOPIC" sheetId="4" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t xml:space="preserve">Property </t>
   </si>
@@ -34,6 +25,9 @@
     <t>Study_ID</t>
   </si>
   <si>
+    <t>STUDY1</t>
+  </si>
+  <si>
     <t>Version</t>
   </si>
   <si>
@@ -73,6 +67,26 @@
     <t>permission uri</t>
   </si>
   <si>
+    <t>STUDY1-DEMO</t>
+  </si>
+  <si>
+    <t>DEMO</t>
+  </si>
+  <si>
+    <t>example-kb:DPL-generic-questionnaire</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>example@example.com</t>
+    </r>
+  </si>
+  <si>
     <t>Public</t>
   </si>
   <si>
@@ -95,45 +109,41 @@
   </si>
   <si>
     <t>topic</t>
-  </si>
-  <si>
-    <t>example-kb:DPL-generic-questionnaire</t>
-  </si>
-  <si>
-    <t>EXAMPLE</t>
-  </si>
-  <si>
-    <t>example@example.com</t>
-  </si>
-  <si>
-    <t>DEMO</t>
-  </si>
-  <si>
-    <t>STUDY1-DEMO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -150,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -173,112 +183,178 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -480,7 +556,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -499,7 +575,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -529,7 +605,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -555,7 +631,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -581,7 +657,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -607,7 +683,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -633,7 +709,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -659,7 +735,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -685,7 +761,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -711,7 +787,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -737,7 +813,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -750,15 +826,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -775,7 +845,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -794,7 +864,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -820,7 +890,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -846,7 +916,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -872,7 +942,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -898,7 +968,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -924,7 +994,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -950,7 +1020,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -976,7 +1046,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1002,7 +1072,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1028,7 +1098,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1041,15 +1111,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1063,7 +1127,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1082,7 +1146,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1112,7 +1176,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1138,7 +1202,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1164,7 +1228,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1190,7 +1254,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1216,7 +1280,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1242,7 +1306,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1268,7 +1332,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1294,7 +1358,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1320,7 +1384,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1333,65 +1397,55 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1719" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
     <col min="3" max="5" width="11.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="13.75" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+    <row r="2" ht="13.75" customHeight="1">
+      <c r="A2" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>25</v>
+      <c r="B2" t="s" s="2">
+        <v>3</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
+    <row r="3" ht="13.75" customHeight="1">
+      <c r="A3" t="s" s="2">
+        <v>4</v>
       </c>
       <c r="B3" s="4">
         <v>5</v>
@@ -1400,61 +1454,61 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="4" ht="13.75" customHeight="1">
+      <c r="A4" t="s" s="2">
         <v>5</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>6</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="5" ht="13.75" customHeight="1">
+      <c r="A5" t="s" s="2">
         <v>7</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>8</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="6" ht="13.75" customHeight="1">
+      <c r="A6" t="s" s="2">
         <v>9</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>10</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" ht="13.75" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" ht="13.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" ht="13.75" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" ht="13.75" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1462,8 +1516,8 @@
       <c r="E10" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05278" bottom="1.05278" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000InfoSheet</oddHeader>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
@@ -1472,68 +1526,130 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="42.83203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="31.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6719" style="5" customWidth="1"/>
+    <col min="2" max="2" width="42.8516" style="5" customWidth="1"/>
+    <col min="3" max="3" width="31.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="65.1640625" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="5"/>
+    <col min="5" max="5" width="22.8516" style="5" customWidth="1"/>
+    <col min="6" max="6" width="65.1719" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="8.85156" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" ht="13.75" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>24</v>
+      <c r="F1" t="s" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" ht="13.75" customHeight="1">
+      <c r="A2" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>19</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" location="" tooltip="" display="example@example.com"/>
   </hyperlinks>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05278" bottom="1.05278" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000FILESTREAM</oddHeader>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
@@ -1542,45 +1658,44 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="8" width="11.5" style="6" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="6"/>
+    <col min="1" max="8" width="11.5" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="8.85156" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="2" t="s">
+    <row r="1" ht="13.75" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H1" t="s" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" ht="13.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1590,7 +1705,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" ht="13.75" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1600,7 +1715,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" ht="13.75" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1610,7 +1725,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" ht="13.75" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1620,7 +1735,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" ht="13.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1630,7 +1745,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" ht="13.75" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1640,7 +1755,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" ht="13.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1650,7 +1765,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" ht="13.75" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1660,7 +1775,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" ht="13.75" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1671,8 +1786,8 @@
       <c r="H10" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05278" bottom="1.05278" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000MESSAGESTREAM</oddHeader>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
@@ -1681,90 +1796,89 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="11.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="7"/>
+    <col min="1" max="5" width="11.5" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
+    <row r="1" ht="13.75" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s" s="2">
         <v>13</v>
       </c>
+      <c r="D1" t="s" s="2">
+        <v>14</v>
+      </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" ht="13.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" ht="13.75" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" ht="13.75" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" ht="13.75" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" ht="13.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" ht="13.75" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" ht="13.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" ht="13.75" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" ht="13.75" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1772,8 +1886,8 @@
       <c r="E10" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05278" bottom="1.05278" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000MESSAGETOPIC</oddHeader>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>

</xml_diff>